<commit_message>
additional learning on Aug26
</commit_message>
<xml_diff>
--- a/CY_Commands.xlsx
+++ b/CY_Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\cy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2C2777-B374-4E02-94A4-B1165C1FDAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE654425-39CC-45FD-8EBD-48EC425A60B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F13F3751-35DC-40E7-802A-A97A9583C87C}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Navigate to URL</t>
   </si>
@@ -127,9 +127,6 @@
     <t>With the help of Jquery selectors, we can retrieve only visible products by using "css_xpath:visible"</t>
   </si>
   <si>
-    <t>should' is the assertion type of "Chai"</t>
-  </si>
-  <si>
     <t>Practice site</t>
   </si>
   <si>
@@ -157,21 +154,12 @@
     <t>should</t>
   </si>
   <si>
-    <t>assertion</t>
-  </si>
-  <si>
     <t>find</t>
   </si>
   <si>
-    <t>search from list of similar locators</t>
-  </si>
-  <si>
     <t>contains</t>
   </si>
   <si>
-    <t>helps finding some specific locator</t>
-  </si>
-  <si>
     <t>cy.get("          ").find("    ")</t>
   </si>
   <si>
@@ -179,6 +167,60 @@
   </si>
   <si>
     <t>cy.get("          ").find("    ").eq(0).contains('        ').click()</t>
+  </si>
+  <si>
+    <t>each</t>
+  </si>
+  <si>
+    <t>Search from list of similar locators</t>
+  </si>
+  <si>
+    <t>Assertion</t>
+  </si>
+  <si>
+    <t>Helps finding some specific locator</t>
+  </si>
+  <si>
+    <t>Helps iterating through an array</t>
+  </si>
+  <si>
+    <t>"should" is the assertion type of "Chai"</t>
+  </si>
+  <si>
+    <t>To resolve the promise, thus refraining from getting 'click()' method deprecated</t>
+  </si>
+  <si>
+    <t>cy.warp(    )</t>
+  </si>
+  <si>
+    <t>wrap</t>
+  </si>
+  <si>
+    <t>Cypress is asynchronous in nature and there is no guarantee in sequence of execution , but Cypress takes care of it.</t>
+  </si>
+  <si>
+    <t>Promise comes with 'resolved', 'rejected' and 'pending'</t>
+  </si>
+  <si>
+    <t>then</t>
+  </si>
+  <si>
+    <t>.then()</t>
+  </si>
+  <si>
+    <t>Wait until promise is resolved(don't rush)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>.text()</t>
+  </si>
+  <si>
+    <t>jQuery command return text content of the selected elements(supported by Cypress after manually resolving promise)</t>
+  </si>
+  <si>
+    <t>Non cypress commands can not resolve promise by themselves, we need to manually resolve it by using then()</t>
   </si>
 </sst>
 </file>
@@ -599,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F97E336-0348-45E1-B449-EAF4E6397907}">
-  <dimension ref="B1:F14"/>
+  <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -644,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -661,7 +703,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -675,18 +717,18 @@
         <v>19</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>12</v>
@@ -694,57 +736,92 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
       <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
       <c r="E11" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -754,7 +831,22 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E14" s="6" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first commit Aug27, 2024
</commit_message>
<xml_diff>
--- a/CY_Commands.xlsx
+++ b/CY_Commands.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\cy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE654425-39CC-45FD-8EBD-48EC425A60B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58655ACD-EAA8-477A-95D6-20E02A0F9CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F13F3751-35DC-40E7-802A-A97A9583C87C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CSS XPATH" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
     <author>DELL</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{3807910C-1E73-48AD-937C-DA253991F676}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{3807910C-1E73-48AD-937C-DA253991F676}">
       <text>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Navigate to URL</t>
   </si>
@@ -163,9 +164,6 @@
     <t>cy.get("          ").find("    ")</t>
   </si>
   <si>
-    <t>cy.get("          ").find("    ").should('have.length)</t>
-  </si>
-  <si>
     <t>cy.get("          ").find("    ").eq(0).contains('        ').click()</t>
   </si>
   <si>
@@ -221,6 +219,90 @@
   </si>
   <si>
     <t>Non cypress commands can not resolve promise by themselves, we need to manually resolve it by using then()</t>
+  </si>
+  <si>
+    <t>Aliasing to reuse locators</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>.click()</t>
+  </si>
+  <si>
+    <t>For clicking on any element</t>
+  </si>
+  <si>
+    <t>For checking checkboxes(.click() also works)</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>.check()</t>
+  </si>
+  <si>
+    <t>For length, text assertion</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>For checkbox assertion</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>should('have.length') ; should('have.text')</t>
+  </si>
+  <si>
+    <t>should('be.checked')</t>
+  </si>
+  <si>
+    <t>cy.get("          ").find("    ").should('have.length')</t>
+  </si>
+  <si>
+    <t>cy.get('#checkBoxOption2').check().should('be.checked').and('have.value','option2')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple assertion </t>
+  </si>
+  <si>
+    <t>Chai js library: 'comparison' --&gt; ('have.   ') ; 'behavioural' --&gt; ('be.   ')</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>#idname</t>
+  </si>
+  <si>
+    <t>tagname#idname</t>
+  </si>
+  <si>
+    <t>classname</t>
+  </si>
+  <si>
+    <t>.classname</t>
+  </si>
+  <si>
+    <t>tagname.classname</t>
+  </si>
+  <si>
+    <t>xpath1</t>
+  </si>
+  <si>
+    <t>xpath2</t>
+  </si>
+  <si>
+    <t>locatorPresent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customized with any attribute </t>
+  </si>
+  <si>
+    <t>tagname[attribute=value]</t>
   </si>
 </sst>
 </file>
@@ -306,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,6 +401,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -640,227 +723,354 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F97E336-0348-45E1-B449-EAF4E6397907}">
-  <dimension ref="B1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F97E336-0348-45E1-B449-EAF4E6397907}">
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.21875" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="96.21875" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="E8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E14" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" location="/" xr:uid="{AE7D4249-0947-4749-8EA9-96795CDE522E}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{30A7341E-4B1C-48BD-934D-28FCB7DE0129}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{C76B4F14-928A-470A-AEA2-32C32708A0A5}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{512A8170-4853-4B08-8007-E135292DE06B}"/>
-    <hyperlink ref="F8" r:id="rId5" xr:uid="{3858BE26-EA35-4F1E-96C5-767C3A53846F}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{EAC20E03-7E98-4A4D-A763-A0902A656652}"/>
-    <hyperlink ref="F11" r:id="rId7" xr:uid="{0794A9F7-BE13-452D-8F16-8F9F30C7AB2A}"/>
+    <hyperlink ref="E2" r:id="rId1" location="/" xr:uid="{AE7D4249-0947-4749-8EA9-96795CDE522E}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{30A7341E-4B1C-48BD-934D-28FCB7DE0129}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{C76B4F14-928A-470A-AEA2-32C32708A0A5}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{512A8170-4853-4B08-8007-E135292DE06B}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{3858BE26-EA35-4F1E-96C5-767C3A53846F}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{EAC20E03-7E98-4A4D-A763-A0902A656652}"/>
+    <hyperlink ref="E11" r:id="rId7" xr:uid="{0794A9F7-BE13-452D-8F16-8F9F30C7AB2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E65070-7DC1-4A23-9043-A7D89B4BF1CB}">
+  <dimension ref="B3:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
second commit Aug27, 2024
</commit_message>
<xml_diff>
--- a/CY_Commands.xlsx
+++ b/CY_Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\cy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58655ACD-EAA8-477A-95D6-20E02A0F9CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525D8542-0362-4ED3-B420-73BDC31A2D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F13F3751-35DC-40E7-802A-A97A9583C87C}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Navigate to URL</t>
   </si>
@@ -233,9 +233,6 @@
     <t>For clicking on any element</t>
   </si>
   <si>
-    <t>For checking checkboxes(.click() also works)</t>
-  </si>
-  <si>
     <t>check</t>
   </si>
   <si>
@@ -303,6 +300,42 @@
   </si>
   <si>
     <t>tagname[attribute=value]</t>
+  </si>
+  <si>
+    <t>For checking checkboxes(.click() also works) and radio buttons</t>
+  </si>
+  <si>
+    <t>Cypress automatically handles pop-ups(alerts) or we can say that Cypress auto accepts alerts/pop ups</t>
+  </si>
+  <si>
+    <t>Cypress can control and manipulate DOM/HTML (Selenium can't do it)</t>
+  </si>
+  <si>
+    <t>Cypress has the capability of firing browser events.</t>
+  </si>
+  <si>
+    <t>We can fire that event through Cypress to get access to the alert.D4D55</t>
+  </si>
+  <si>
+    <t>window:alert' or 'window:confirm' is the event which gets fired when an alert is opened.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In HTML, Static dowdown will always have 'select' tagname. </t>
+  </si>
+  <si>
+    <t>In HTML, 'href="www.xyz.com" target="_blank"'; will always open link in new tab</t>
+  </si>
+  <si>
+    <t>We can use 'jQuery' at runtime to make changes in DOM</t>
+  </si>
+  <si>
+    <t>Cypress directly can't switch to new window/tab and perform actions</t>
+  </si>
+  <si>
+    <t>.invoke('removeAttr','target')</t>
+  </si>
+  <si>
+    <t>To remove an attribute from DOM in run-time</t>
   </si>
 </sst>
 </file>
@@ -355,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +407,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -388,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -402,6 +447,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -411,6 +459,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFFCC"/>
+      <color rgb="FF99CCFF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFCC00CC"/>
@@ -724,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F97E336-0348-45E1-B449-EAF4E6397907}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,6 +863,9 @@
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -822,7 +875,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>26</v>
@@ -846,6 +902,9 @@
       <c r="B8" t="s">
         <v>35</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="E8" s="7" t="s">
         <v>27</v>
       </c>
@@ -874,6 +933,9 @@
       <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -885,9 +947,6 @@
       <c r="C11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
       <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
@@ -903,74 +962,110 @@
         <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>40</v>
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
         <v>62</v>
       </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
-        <v>69</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1030,43 +1125,43 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>71</v>
-      </c>
-      <c r="D13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>74</v>
-      </c>
-      <c r="D14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
         <v>79</v>
-      </c>
-      <c r="C16" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>